<commit_message>
first attempt fix conflicts
only changed 2 files
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/energy-inputs-copper-maths.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/energy-inputs-copper-maths.xlsx
@@ -8,22 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5291A041-EC3C-4F9F-99D3-C626CA2744EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952A9CC6-E924-498D-95D1-EED9768FACF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{5A880DFA-5001-4668-A9E5-FAA5270211BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="oregradeovertime" sheetId="2" r:id="rId2"/>
     <sheet name="pyrovshydro" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">pyrovshydro!$A$2:$A$29</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">pyrovshydro!$E$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">pyrovshydro!$E$2:$E$29</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">pyrovshydro!$F$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">pyrovshydro!$F$2:$F$29</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1317,6 +1310,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="628521952"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1903,7 +1897,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$2</c:f>
+              <c:f>oregradeovertime!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1926,7 +1920,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$3:$A$23</c:f>
+              <c:f>oregradeovertime!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1998,7 +1992,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$3:$B$23</c:f>
+              <c:f>oregradeovertime!$B$3:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2068,7 +2062,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$2</c:f>
+              <c:f>oregradeovertime!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2091,7 +2085,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$3:$A$23</c:f>
+              <c:f>oregradeovertime!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2163,7 +2157,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$C$3:$C$23</c:f>
+              <c:f>oregradeovertime!$C$3:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2245,7 +2239,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$2</c:f>
+              <c:f>oregradeovertime!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2268,7 +2262,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$3:$A$23</c:f>
+              <c:f>oregradeovertime!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2340,7 +2334,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$D$3:$D$23</c:f>
+              <c:f>oregradeovertime!$D$3:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2422,7 +2416,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$E$2</c:f>
+              <c:f>oregradeovertime!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2445,7 +2439,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$3:$A$23</c:f>
+              <c:f>oregradeovertime!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2517,7 +2511,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$E$3:$E$23</c:f>
+              <c:f>oregradeovertime!$E$3:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2599,7 +2593,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$G$2</c:f>
+              <c:f>oregradeovertime!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2622,7 +2616,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$3:$A$23</c:f>
+              <c:f>oregradeovertime!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2694,7 +2688,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$G$3:$G$23</c:f>
+              <c:f>oregradeovertime!$G$3:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3516,7 +3510,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -6958,7 +6952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8692A31-05C2-475A-9FAD-02E1D54F89A5}">
   <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -7224,7 +7218,7 @@
         <v>0.9741770462161411</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N4:N23" si="6">(277.77777/1000)*36.529*M5^(-0.351)</f>
+        <f t="shared" ref="N5:N23" si="6">(277.77777/1000)*36.529*M5^(-0.351)</f>
         <v>10.240552070330814</v>
       </c>
       <c r="O5">
@@ -8394,11 +8388,11 @@
         <v>1996</v>
       </c>
       <c r="S27">
-        <f t="shared" ref="S27:S47" si="7">5.898*S4^(-0.199)</f>
+        <f t="shared" ref="S27:S46" si="7">5.898*S4^(-0.199)</f>
         <v>5.0935186291701626</v>
       </c>
       <c r="T27">
-        <f t="shared" ref="T27:U47" si="8">(277.77777/1000)*36.529*T4^(-0.351)</f>
+        <f t="shared" ref="T27:U46" si="8">(277.77777/1000)*36.529*T4^(-0.351)</f>
         <v>12.59585342250984</v>
       </c>
       <c r="U27">
@@ -8484,7 +8478,7 @@
         <v>1999</v>
       </c>
       <c r="R30">
-        <f t="shared" ref="R27:R47" si="9">5.55*R7^(-0.634)</f>
+        <f t="shared" ref="R30:R46" si="9">5.55*R7^(-0.634)</f>
         <v>4.4741520423600889</v>
       </c>
       <c r="S30">
@@ -9539,7 +9533,7 @@
         <v>8533.0191916188196</v>
       </c>
       <c r="C2">
-        <f>D2-B2</f>
+        <f t="shared" ref="C2:C29" si="0">D2-B2</f>
         <v>796.02900473500085</v>
       </c>
       <c r="D2">
@@ -9562,18 +9556,18 @@
         <v>8849.7838369512992</v>
       </c>
       <c r="C3">
-        <f>D3-B3</f>
+        <f t="shared" si="0"/>
         <v>995.44799505913033</v>
       </c>
       <c r="D3">
         <v>9845.2318320104296</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E29" si="0">B3/$D3</f>
+        <f t="shared" ref="E3:E29" si="1">B3/$D3</f>
         <v>0.89889034488527053</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F29" si="1">C3/$D3</f>
+        <f t="shared" ref="F3:F29" si="2">C3/$D3</f>
         <v>0.10110965511472943</v>
       </c>
     </row>
@@ -9585,18 +9579,18 @@
         <v>9445.5703730814093</v>
       </c>
       <c r="C4">
-        <f>D4-B4</f>
+        <f t="shared" si="0"/>
         <v>1392.9135119060902</v>
       </c>
       <c r="D4">
         <v>10838.4838849875</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.87148446898228726</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12851553101771271</v>
       </c>
     </row>
@@ -9608,18 +9602,18 @@
         <v>9523.5263169933805</v>
       </c>
       <c r="C5">
-        <f>D5-B5</f>
+        <f t="shared" si="0"/>
         <v>1790.9280142736188</v>
       </c>
       <c r="D5">
         <v>11314.454331266999</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84171326677907321</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.15828673322092676</v>
       </c>
     </row>
@@ -9631,18 +9625,18 @@
         <v>10039.572706269801</v>
       </c>
       <c r="C6">
-        <f>D6-B6</f>
+        <f t="shared" si="0"/>
         <v>1989.7980190772996</v>
       </c>
       <c r="D6">
         <v>12029.3707253471</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83458835341365001</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16541164658635002</v>
       </c>
     </row>
@@ -9654,18 +9648,18 @@
         <v>10236.795754511901</v>
       </c>
       <c r="C7">
-        <f>D7-B7</f>
+        <f t="shared" si="0"/>
         <v>2348.4228103484002</v>
       </c>
       <c r="D7">
         <v>12585.218564860301</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.81339832929834632</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18660167070165368</v>
       </c>
     </row>
@@ -9677,7 +9671,7 @@
         <v>10713.0406935517</v>
       </c>
       <c r="C8">
-        <f>D8-B8</f>
+        <f t="shared" si="0"/>
         <v>1913.8115607200398</v>
       </c>
       <c r="D8">
@@ -9685,11 +9679,11 @@
         <v>12626.85225427174</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84843320233888175</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.15156679766111825</v>
       </c>
     </row>
@@ -9701,18 +9695,18 @@
         <v>10830.935334080499</v>
       </c>
       <c r="C9">
-        <f>D9-B9</f>
+        <f t="shared" si="0"/>
         <v>2586.9570190086015</v>
       </c>
       <c r="D9">
         <v>13417.892353089101</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80720094103206708</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1927990589679329</v>
       </c>
     </row>
@@ -9724,18 +9718,18 @@
         <v>10670.082576572</v>
       </c>
       <c r="C10">
-        <f>D10-B10</f>
+        <f t="shared" si="0"/>
         <v>2666.6971658622006</v>
       </c>
       <c r="D10">
         <v>13336.779742434201</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80004939592895452</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19995060407104545</v>
       </c>
     </row>
@@ -9747,18 +9741,18 @@
         <v>10787.977217100901</v>
       </c>
       <c r="C11">
-        <f>D11-B11</f>
+        <f t="shared" si="0"/>
         <v>2746.1628199555998</v>
       </c>
       <c r="D11">
         <v>13534.140037056501</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.79709366000081272</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.20290633999918731</v>
       </c>
     </row>
@@ -9770,18 +9764,18 @@
         <v>11741.839558981599</v>
       </c>
       <c r="C12">
-        <f>D12-B12</f>
+        <f t="shared" si="0"/>
         <v>2666.4226731020008</v>
       </c>
       <c r="D12">
         <v>14408.2622320836</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.81493794115125529</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18506205884874469</v>
       </c>
     </row>
@@ -9793,18 +9787,18 @@
         <v>12058.604204314101</v>
       </c>
       <c r="C13">
-        <f>D13-B13</f>
+        <f t="shared" si="0"/>
         <v>2666.422673101999</v>
       </c>
       <c r="D13">
         <v>14725.0268774161</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.81891899449151329</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18108100550848666</v>
       </c>
     </row>
@@ -9816,18 +9810,18 @@
         <v>11977.491593659201</v>
       </c>
       <c r="C14">
-        <f>D14-B14</f>
+        <f t="shared" si="0"/>
         <v>2825.6284740489991</v>
       </c>
       <c r="D14">
         <v>14803.1200677082</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80911939772664021</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19088060227335976</v>
       </c>
     </row>
@@ -9839,18 +9833,18 @@
         <v>12294.3934853718</v>
       </c>
       <c r="C15">
-        <f>D15-B15</f>
+        <f t="shared" si="0"/>
         <v>3024.7729716127997</v>
       </c>
       <c r="D15">
         <v>15319.1664569846</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80254976795857658</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19745023204142342</v>
       </c>
     </row>
@@ -9862,18 +9856,18 @@
         <v>12292.883775190399</v>
       </c>
       <c r="C16">
-        <f>D16-B16</f>
+        <f t="shared" si="0"/>
         <v>3024.7729716129015</v>
       </c>
       <c r="D16">
         <v>15317.656746803301</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80253030723879137</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19746969276120857</v>
       </c>
     </row>
@@ -9885,18 +9879,18 @@
         <v>12490.518562572899</v>
       </c>
       <c r="C17">
-        <f>D17-B17</f>
+        <f t="shared" si="0"/>
         <v>3303.2458768900015</v>
       </c>
       <c r="D17">
         <v>15793.764439462901</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.79085126351280854</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.20914873648719146</v>
       </c>
     </row>
@@ -9908,18 +9902,18 @@
         <v>12488.8716060113</v>
       </c>
       <c r="C18">
-        <f>D18-B18</f>
+        <f t="shared" si="0"/>
         <v>3303.1283939886998</v>
       </c>
       <c r="D18">
         <v>15792</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.79083533472715928</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.20916466527284067</v>
       </c>
     </row>
@@ -9931,18 +9925,18 @@
         <v>12288.217398266101</v>
       </c>
       <c r="C19">
-        <f>D19-B19</f>
+        <f t="shared" si="0"/>
         <v>3502.3903744538002</v>
       </c>
       <c r="D19">
         <v>15790.607772719901</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.77819787402327956</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.22180212597672042</v>
       </c>
     </row>
@@ -9954,18 +9948,18 @@
         <v>12923.393645492501</v>
       </c>
       <c r="C20">
-        <f>D20-B20</f>
+        <f t="shared" si="0"/>
         <v>3542.3290710708006</v>
       </c>
       <c r="D20">
         <v>16465.722716563301</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.78486646884272626</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.21513353115727371</v>
       </c>
     </row>
@@ -9977,18 +9971,18 @@
         <v>14235.6062858842</v>
       </c>
       <c r="C21">
-        <f>D21-B21</f>
+        <f t="shared" si="0"/>
         <v>3741.0618294942014</v>
       </c>
       <c r="D21">
         <v>17976.668115378401</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.7918934807338488</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2081065192661512</v>
       </c>
     </row>
@@ -10000,18 +9994,18 @@
         <v>14313.424983416</v>
       </c>
       <c r="C22">
-        <f>D22-B22</f>
+        <f t="shared" si="0"/>
         <v>3940.3435734382983</v>
       </c>
       <c r="D22">
         <v>18253.768556854298</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.78413533834586191</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.21586466165413812</v>
       </c>
     </row>
@@ -10023,18 +10017,18 @@
         <v>15028.478623876201</v>
       </c>
       <c r="C23">
-        <f>D23-B23</f>
+        <f t="shared" si="0"/>
         <v>3940.0690806779985</v>
       </c>
       <c r="D23">
         <v>18968.547704554199</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.79228409354017026</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.20771590645982976</v>
       </c>
     </row>
@@ -10046,18 +10040,18 @@
         <v>16300.4780748907</v>
       </c>
       <c r="C24">
-        <f>D24-B24</f>
+        <f t="shared" si="0"/>
         <v>3860.6034265847011</v>
       </c>
       <c r="D24">
         <v>20161.081501475401</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80851208670020114</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19148791329979892</v>
       </c>
     </row>
@@ -10069,18 +10063,18 @@
         <v>16060.434156049099</v>
       </c>
       <c r="C25">
-        <f>D25-B25</f>
+        <f t="shared" si="0"/>
         <v>3781.0005261111019</v>
       </c>
       <c r="D25">
         <v>19841.434682160201</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80943915665984234</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19056084334015772</v>
       </c>
     </row>
@@ -10092,18 +10086,18 @@
         <v>16496.465905711699</v>
       </c>
       <c r="C26">
-        <f>D26-B26</f>
+        <f t="shared" si="0"/>
         <v>3860.6034265846029</v>
       </c>
       <c r="D26">
         <v>20357.069332296302</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.81035563795718912</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1896443620428109</v>
       </c>
     </row>
@@ -10115,7 +10109,7 @@
         <v>16335.7503945833</v>
       </c>
       <c r="C27">
-        <f>D27-B27</f>
+        <f t="shared" si="0"/>
         <v>4079.511402886752</v>
       </c>
       <c r="D27">
@@ -10123,11 +10117,11 @@
         <v>20415.261797470052</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80017344654417788</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19982655345582209</v>
       </c>
     </row>
@@ -10139,18 +10133,18 @@
         <v>16413.7063384953</v>
       </c>
       <c r="C28">
-        <f>D28-B28</f>
+        <f t="shared" si="0"/>
         <v>4059.7479241485016</v>
       </c>
       <c r="D28">
         <v>20473.454262643801</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80170674317738444</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19829325682261562</v>
       </c>
     </row>
@@ -10162,18 +10156,18 @@
         <v>17088.821282338598</v>
       </c>
       <c r="C29">
-        <f>D29-B29</f>
+        <f t="shared" si="0"/>
         <v>3821.0764691082004</v>
       </c>
       <c r="D29">
         <v>20909.897751446799</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.81725991611585891</v>
       </c>
       <c r="F29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18274008388414106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
copper energy redo work
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/energy-inputs-copper-maths.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/energy-inputs-copper-maths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6F8453-B817-4609-A0F4-7B36663EB923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BB10B9-276C-4008-A730-DB8D5267E939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5A880DFA-5001-4668-A9E5-FAA5270211BD}"/>
+    <workbookView xWindow="41655" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{5A880DFA-5001-4668-A9E5-FAA5270211BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -256,14 +256,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6617,15 +6617,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6972,17 +6972,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>31</v>
       </c>
       <c r="M1" t="s">
@@ -6997,7 +6997,7 @@
       <c r="Q1" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -7023,13 +7023,13 @@
       <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>21</v>
       </c>
       <c r="M2" t="s">
@@ -7085,14 +7085,14 @@
         <f>F3*E3</f>
         <v>0.91866666666666663</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>0.01</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="6">
         <f>36.529*I3^(-0.351)</f>
         <v>183.92373738413374</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <f>15.697*I3^(-0.573)</f>
         <v>219.69322202422373</v>
       </c>
@@ -7142,14 +7142,14 @@
         <f t="shared" ref="D4:D36" si="0">C4*(277.77777/1000)</f>
         <v>6.4444442639999995</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>0.1</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <f t="shared" ref="J4:J18" si="1">36.529*I4^(-0.351)</f>
         <v>81.966762793860667</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <f t="shared" ref="K4:K18" si="2">15.697*I4^(-0.573)</f>
         <v>58.724139041064191</v>
       </c>
@@ -7199,14 +7199,14 @@
         <f t="shared" si="0"/>
         <v>2.8055554769999995</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>0.2</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <f t="shared" si="1"/>
         <v>64.265257920016879</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <f t="shared" si="2"/>
         <v>39.475393764145572</v>
       </c>
@@ -7256,14 +7256,14 @@
         <f t="shared" si="0"/>
         <v>5.9166665009999999</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>0.3</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <f t="shared" si="1"/>
         <v>55.740161531221595</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <f t="shared" si="2"/>
         <v>31.291485386920399</v>
       </c>
@@ -7313,14 +7313,14 @@
         <f t="shared" si="0"/>
         <v>5.3888887379999995</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>0.4</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <f t="shared" si="1"/>
         <v>50.386562000904483</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <f t="shared" si="2"/>
         <v>26.536050392235836</v>
       </c>
@@ -7373,14 +7373,14 @@
         <f t="shared" si="0"/>
         <v>7.5555553439999992</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>0.5</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <f t="shared" si="1"/>
         <v>46.590708183625537</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <f t="shared" si="2"/>
         <v>23.351073228934425</v>
       </c>
@@ -7433,14 +7433,14 @@
         <f t="shared" si="0"/>
         <v>4.9166665289999996</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>0.6</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <f t="shared" si="1"/>
         <v>43.702541557194003</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <f t="shared" si="2"/>
         <v>21.034683986595656</v>
       </c>
@@ -7493,14 +7493,14 @@
         <f t="shared" si="0"/>
         <v>5.2222220759999995</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>0.7</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="6">
         <f t="shared" si="1"/>
         <v>41.400765499835678</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <f t="shared" si="2"/>
         <v>19.256416967953527</v>
       </c>
@@ -7553,14 +7553,14 @@
         <f t="shared" si="0"/>
         <v>11.277777462</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>0.8</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="6">
         <f t="shared" si="1"/>
         <v>39.505102950504515</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <f t="shared" si="2"/>
         <v>17.837997376959692</v>
       </c>
@@ -7616,14 +7616,14 @@
         <f t="shared" si="0"/>
         <v>10.361110820999999</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>0.9</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <f t="shared" si="1"/>
         <v>37.905188659706205</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <f t="shared" si="2"/>
         <v>16.673842711174611</v>
       </c>
@@ -7690,14 +7690,14 @@
         <f>F13*E13</f>
         <v>0.65549999999999997</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <v>1</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="6">
         <f t="shared" si="1"/>
         <v>36.529000000000003</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <f t="shared" si="2"/>
         <v>15.696999999999999</v>
       </c>
@@ -7750,14 +7750,14 @@
         <f t="shared" si="0"/>
         <v>5.5555553999999994</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="6">
         <f t="shared" si="1"/>
         <v>35.32717834761295</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <f t="shared" si="2"/>
         <v>14.862732098302478</v>
       </c>
@@ -7824,14 +7824,14 @@
         <f>F15*E15</f>
         <v>7.2310000000000016</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <v>1.2</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="6">
         <f t="shared" si="1"/>
         <v>34.264560526766218</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <f t="shared" si="2"/>
         <v>14.139882621260533</v>
       </c>
@@ -7884,14 +7884,14 @@
         <f t="shared" si="0"/>
         <v>4.7499998669999997</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <v>1.3</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="6">
         <f t="shared" si="1"/>
         <v>33.315295266471068</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <f t="shared" si="2"/>
         <v>13.506011569251946</v>
       </c>
@@ -7944,14 +7944,14 @@
         <f t="shared" si="0"/>
         <v>4.1666665499999995</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <v>1.4</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="6">
         <f t="shared" si="1"/>
         <v>32.459874981574345</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <f t="shared" si="2"/>
         <v>12.944500416855565</v>
       </c>
@@ -8004,14 +8004,14 @@
         <f t="shared" si="0"/>
         <v>7.7499997829999989</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="6">
         <v>1.5</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="6">
         <f t="shared" si="1"/>
         <v>31.683251985203562</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="6">
         <f t="shared" si="2"/>
         <v>12.442749755788808</v>
       </c>
@@ -8665,7 +8665,7 @@
         <f>F35*AVERAGE(C27:C30,C32,C12)</f>
         <v>12.266999999999998</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H35" s="5">
         <f>G34*277.77777/1000</f>
         <v>5.8533794657350002</v>
       </c>
@@ -8694,7 +8694,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="5" t="s">
         <v>28</v>
       </c>
       <c r="Q36">
@@ -8951,7 +8951,7 @@
   <dimension ref="A2:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F24"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9489,10 +9489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64978AA1-20C7-4AF0-8552-AAAE88FF8E96}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9505,10 +9505,7 @@
     <col min="6" max="6" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>43</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>46</v>
       </c>
@@ -9524,8 +9521,11 @@
       <c r="F1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1994</v>
       </c>
@@ -9548,7 +9548,7 @@
         <v>8.5327997881511866E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1995</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>0.10110965511472943</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>1996</v>
       </c>
@@ -9594,7 +9594,7 @@
         <v>0.12851553101771271</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>1997</v>
       </c>
@@ -9617,7 +9617,7 @@
         <v>0.15828673322092676</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>1998</v>
       </c>
@@ -9640,7 +9640,7 @@
         <v>0.16541164658635002</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>1999</v>
       </c>
@@ -9663,7 +9663,7 @@
         <v>0.18660167070165368</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>2000</v>
       </c>
@@ -9687,7 +9687,7 @@
         <v>0.15156679766111825</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>2001</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>0.1927990589679329</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>2002</v>
       </c>
@@ -9733,7 +9733,7 @@
         <v>0.19995060407104545</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>2003</v>
       </c>
@@ -9756,7 +9756,7 @@
         <v>0.20290633999918731</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>2004</v>
       </c>
@@ -9779,7 +9779,7 @@
         <v>0.18506205884874469</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>2005</v>
       </c>
@@ -9802,7 +9802,7 @@
         <v>0.18108100550848666</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>2006</v>
       </c>
@@ -9825,7 +9825,7 @@
         <v>0.19088060227335976</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>2007</v>
       </c>
@@ -9848,7 +9848,7 @@
         <v>0.19745023204142342</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>2008</v>
       </c>
@@ -10169,6 +10169,151 @@
       <c r="F29" s="2">
         <f t="shared" si="2"/>
         <v>0.18274008388414106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="3">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="3">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="3">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="3">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="3">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="3">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="3">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="3">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="3">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="3">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="3">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="3">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="3">
+        <v>2050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>